<commit_message>
updates and syntax changes
</commit_message>
<xml_diff>
--- a/threatmodel-fractus.xlsx
+++ b/threatmodel-fractus.xlsx
@@ -22,19 +22,19 @@
     <t>question</t>
   </si>
   <si>
+    <t>severity</t>
+  </si>
+  <si>
     <t>why</t>
   </si>
   <si>
-    <t>severity</t>
-  </si>
-  <si>
     <t>Does the service provide direct internet egress functionality?</t>
   </si>
   <si>
     <t>Does the service introduce a network entry point (ingress access) from the internet?</t>
   </si>
   <si>
-    <t>Can the service be made publicly accessible?</t>
+    <t>Can the service resources be made publicly accessible?</t>
   </si>
   <si>
     <t>Does the service expand or elevate administrative/privileged permissions to other services?</t>
@@ -61,6 +61,18 @@
     <t>Does the service have any 3rd party compliance attestations/certifications?</t>
   </si>
   <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Critical</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
     <t>Direct internet access functionality may bypass centralized network logging, monitoring, and visibility resulting in data exfiltration.</t>
   </si>
   <si>
@@ -92,18 +104,6 @@
   </si>
   <si>
     <t>Cloud adoption includes a shared responsibility model. That responsibility is governed via a legally binding contract by both parties. The contract ensures that the cloud provider is responsible for maintaining an adequate level of security. To quantify that 'third-party trust', independent assessments by reputable third-party organizations can provide increased assurance that a cloud provider is meeting the expectations of their service delivery and security expectations.</t>
-  </si>
-  <si>
-    <t>High</t>
-  </si>
-  <si>
-    <t>Critical</t>
-  </si>
-  <si>
-    <t>Medium</t>
-  </si>
-  <si>
-    <t>Low</t>
   </si>
 </sst>
 </file>
@@ -492,7 +492,7 @@
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -503,10 +503,10 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -517,10 +517,10 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -531,10 +531,10 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -545,10 +545,10 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -559,10 +559,10 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -573,10 +573,10 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -587,10 +587,10 @@
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -601,10 +601,10 @@
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -615,10 +615,10 @@
         <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -629,10 +629,10 @@
         <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>